<commit_message>
commit for run 1 of multi-thread refactoring
</commit_message>
<xml_diff>
--- a/docs/Optimizing Imports - Leveraging Multiple Threads.xlsx
+++ b/docs/Optimizing Imports - Leveraging Multiple Threads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/code/ForceDrawnGraphs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC8E1A7-6683-604F-8F9A-464E0606D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0980AE-1522-754C-BDA9-20864651B988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{DB16906F-C7FB-0A4C-9779-A92B59904945}"/>
   </bookViews>
@@ -323,7 +323,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{B962B3B8-8B02-B344-B170-4AE9FC0962B7}" name="process2" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/james/Documents/code/ForceDrawnGraphs/src/main/resources/logs/process.log" comma="1">
+    <textPr sourceFile="/Users/james/Documents/code/ForceDrawnGraphs/src/main/resources/logs/process.log" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -560,6 +560,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -692,14 +695,14 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2339,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4645FB-DBB7-F54E-8FDE-4BFF0061D23B}">
   <dimension ref="A1:BBK60"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B60" sqref="B60:H60"/>
     </sheetView>
   </sheetViews>
@@ -24961,10 +24964,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBDCE78-AA5D-3648-9A62-92656F87868B}">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A2:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24976,12 +24979,12 @@
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" s="11" t="s">
         <v>60</v>
       </c>
@@ -24998,7 +25001,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>52</v>
       </c>
@@ -25027,7 +25030,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="14">
         <v>2</v>
       </c>
@@ -25056,8 +25059,9 @@
         <f>I5-C5</f>
         <v>1763578</v>
       </c>
+      <c r="K5" s="21"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="14">
         <v>4</v>
       </c>
@@ -25087,7 +25091,7 @@
         <v>1741221</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="14">
         <v>5</v>
       </c>
@@ -25117,7 +25121,7 @@
         <v>1735770</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
         <v>52</v>
       </c>
@@ -25140,8 +25144,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="str">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="20" t="str">
         <f>" 2  - " &amp; I5-C5 &amp; " ms."</f>
         <v xml:space="preserve"> 2  - 1763578 ms.</v>
       </c>
@@ -25170,8 +25174,8 @@
         <v>1763578</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="str">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="20" t="str">
         <f>" 4 - " &amp; I6-C6 &amp; " ms."</f>
         <v xml:space="preserve"> 4 - 1741221 ms.</v>
       </c>
@@ -25200,8 +25204,8 @@
         <v>1741221</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="21" t="str">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="20" t="str">
         <f>" 5  - " &amp; I7-C7 &amp; " ms."</f>
         <v xml:space="preserve"> 5  - 1735770 ms.</v>
       </c>
@@ -25210,28 +25214,25 @@
         <v>222939</v>
       </c>
       <c r="D13" s="16">
-        <f t="shared" ref="D12:D13" si="0">E7-C7</f>
+        <f t="shared" ref="D13" si="0">E7-C7</f>
         <v>253100</v>
       </c>
       <c r="E13" s="16">
-        <f t="shared" ref="E12:E13" si="1">F7-C7</f>
+        <f t="shared" ref="E13" si="1">F7-C7</f>
         <v>253149</v>
       </c>
       <c r="F13" s="16">
-        <f t="shared" ref="F12:F13" si="2">G7-C7</f>
+        <f t="shared" ref="F13" si="2">G7-C7</f>
         <v>982024</v>
       </c>
       <c r="G13" s="16">
-        <f t="shared" ref="G12:G13" si="3">H7-C7</f>
+        <f t="shared" ref="G13" si="3">H7-C7</f>
         <v>1735770</v>
       </c>
       <c r="H13" s="16">
-        <f t="shared" ref="H12:H13" si="4">I7-C7</f>
+        <f t="shared" ref="H13" si="4">I7-C7</f>
         <v>1735770</v>
       </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final cleanups to PR
</commit_message>
<xml_diff>
--- a/docs/Optimizing Imports - Leveraging Multiple Threads.xlsx
+++ b/docs/Optimizing Imports - Leveraging Multiple Threads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/code/ForceDrawnGraphs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10AC81E-8548-304E-B476-D5765A2ABE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FFB882-4522-4343-8BD3-19EF09479B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36180" yWindow="-2780" windowWidth="40900" windowHeight="27980" activeTab="5" xr2:uid="{DB16906F-C7FB-0A4C-9779-A92B59904945}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{DB16906F-C7FB-0A4C-9779-A92B59904945}"/>
   </bookViews>
   <sheets>
     <sheet name="Run2 - Single Thread RawDat" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{19630697-9D9B-9443-99DA-7CE668A7D706}" name="process3" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/james/Documents/code/ForceDrawnGraphs/src/main/resources/logs/process.log" comma="1">
+    <textPr sourceFile="/Users/james/Documents/code/ForceDrawnGraphs/src/main/resources/logs/process.log" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -822,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -910,13 +910,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -2151,6 +2144,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
           <c:val>
             <c:numRef>
               <c:f>'All Results'!$D$23:$I$23</c:f>
@@ -2199,6 +2195,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="63500"/>
+          </c:spPr>
           <c:val>
             <c:numRef>
               <c:f>'All Results'!$D$24:$I$24</c:f>
@@ -2562,6 +2561,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="95250"/>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>'All Results'!$D$14:$I$14</c:f>
@@ -2636,6 +2638,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="95250"/>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>'All Results'!$D$14:$I$14</c:f>
@@ -3581,15 +3586,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>797441</xdr:colOff>
+      <xdr:colOff>797440</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>59070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>49985</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>142050</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>514864</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>137297</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -54482,15 +54487,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A23B8EE-0D6F-D047-8A1C-34D6FD684215}">
   <dimension ref="B3:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="37" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="AB106" sqref="AB106"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="37" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="AP88" sqref="AP88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -54498,22 +54502,22 @@
       <c r="B3" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="18" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="18" t="s">
@@ -54521,17 +54525,17 @@
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="49"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="49" t="str">
+      <c r="B5" s="44" t="str">
         <f>"1 MT - " &amp; I5-C5 &amp; "ms."</f>
         <v>1 MT - 815617ms.</v>
       </c>
@@ -54558,7 +54562,7 @@
       </c>
     </row>
     <row r="6" spans="2:9">
-      <c r="B6" s="49" t="str">
+      <c r="B6" s="44" t="str">
         <f>"2 MT - " &amp; I6-C6 &amp; "ms."</f>
         <v>2 MT - 776266ms.</v>
       </c>
@@ -54585,7 +54589,7 @@
       </c>
     </row>
     <row r="7" spans="2:9">
-      <c r="B7" s="49" t="str">
+      <c r="B7" s="44" t="str">
         <f>"3 MT - " &amp; I7-C7 &amp; "ms."</f>
         <v>3 MT - 781995ms.</v>
       </c>
@@ -54612,7 +54616,7 @@
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="49" t="str">
+      <c r="B8" s="44" t="str">
         <f>"4 MT - " &amp; I8-C8 &amp; "ms."</f>
         <v>4 MT - 772267ms.</v>
       </c>
@@ -54639,7 +54643,7 @@
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="49" t="str">
+      <c r="B9" s="44" t="str">
         <f>"5 MT - " &amp; I9-C9 &amp; "ms."</f>
         <v>5 MT - 778790ms.</v>
       </c>
@@ -54666,7 +54670,7 @@
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="49" t="str">
+      <c r="B10" s="44" t="str">
         <f>"2 ST - " &amp; I10-C10 &amp; "ms."</f>
         <v>2 ST - 1763578ms.</v>
       </c>
@@ -54693,7 +54697,7 @@
       </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="49" t="str">
+      <c r="B11" s="44" t="str">
         <f>"4 ST - " &amp; I11-C11 &amp; "ms."</f>
         <v>4 ST - 1741221ms.</v>
       </c>
@@ -54720,7 +54724,7 @@
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="49" t="str">
+      <c r="B12" s="44" t="str">
         <f>"5 ST - " &amp; I12-C12 &amp; "ms."</f>
         <v>5 ST - 1735770ms.</v>
       </c>
@@ -54748,32 +54752,32 @@
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="12"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="45" t="s">
+      <c r="H14" s="18" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="18" t="s">
@@ -54781,11 +54785,11 @@
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="49" t="str">
+      <c r="B15" s="44" t="str">
         <f>"1 MT - " &amp; I5-C5 &amp; "ms."</f>
         <v>1 MT - 815617ms.</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="16">
         <f>D5-C5</f>
         <v>178</v>
@@ -54812,11 +54816,11 @@
       </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="49" t="str">
+      <c r="B16" s="44" t="str">
         <f>"2 MT - " &amp; I6-C6 &amp; "ms."</f>
         <v>2 MT - 776266ms.</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="16">
         <f t="shared" ref="D16:D22" si="0">D6-C6</f>
         <v>192</v>
@@ -54843,11 +54847,11 @@
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="49" t="str">
+      <c r="B17" s="44" t="str">
         <f>"3 MT - " &amp; I7-C7 &amp; "ms."</f>
         <v>3 MT - 781995ms.</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="16">
         <f t="shared" si="0"/>
         <v>201</v>
@@ -54874,11 +54878,11 @@
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="49" t="str">
+      <c r="B18" s="44" t="str">
         <f>"4 MT - " &amp; I8-C8 &amp; "ms."</f>
         <v>4 MT - 772267ms.</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="16">
         <f t="shared" si="0"/>
         <v>260</v>
@@ -54905,11 +54909,11 @@
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="49" t="str">
+      <c r="B19" s="44" t="str">
         <f>"5 MT - " &amp; I9-C9 &amp; "ms."</f>
         <v>5 MT - 778790ms.</v>
       </c>
-      <c r="C19" s="44"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="16">
         <f t="shared" si="0"/>
         <v>226</v>
@@ -54936,11 +54940,11 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="49" t="str">
+      <c r="B20" s="44" t="str">
         <f>"2 ST - " &amp; I10-C10 &amp; "ms."</f>
         <v>2 ST - 1763578ms.</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="16">
         <f t="shared" si="0"/>
         <v>256737</v>
@@ -54967,11 +54971,11 @@
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="49" t="str">
+      <c r="B21" s="44" t="str">
         <f>"4 ST - " &amp; I11-C11 &amp; "ms."</f>
         <v>4 ST - 1741221ms.</v>
       </c>
-      <c r="C21" s="44"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="16">
         <f t="shared" si="0"/>
         <v>254297</v>
@@ -54998,11 +55002,11 @@
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="49" t="str">
+      <c r="B22" s="44" t="str">
         <f>"5 ST - " &amp; I12-C12 &amp; "ms."</f>
         <v>5 ST - 1735770ms.</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="16">
         <f t="shared" si="0"/>
         <v>253149</v>
@@ -55029,11 +55033,11 @@
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="49" t="str">
+      <c r="B23" s="44" t="str">
         <f>"Avg Multi-Threaded - " &amp; (SUM(I15:I19)/5) &amp; "ms."</f>
         <v>Avg Multi-Threaded - 784987ms.</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="16">
         <f>(SUM(D15:D19)/5)</f>
         <v>211.4</v>
@@ -55060,33 +55064,33 @@
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="49" t="str">
+      <c r="B24" s="44" t="str">
         <f>"Avg Single-Threaded - " &amp; ROUNDDOWN((SUM(I20:I22)/3), 0)  &amp; "ms."</f>
         <v>Avg Single-Threaded - 1746856ms.</v>
       </c>
-      <c r="C24" s="44"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="16">
-        <f>(SUM(D20:D22)/3)</f>
+        <f t="shared" ref="D24:I24" si="7">(SUM(D20:D22)/3)</f>
         <v>254727.66666666666</v>
       </c>
       <c r="E24" s="16">
-        <f>(SUM(E20:E22)/3)</f>
+        <f t="shared" si="7"/>
         <v>254682</v>
       </c>
-      <c r="F24" s="50">
-        <f>(SUM(F20:F22)/3)</f>
+      <c r="F24" s="45">
+        <f t="shared" si="7"/>
         <v>224337.66666666666</v>
       </c>
       <c r="G24" s="16">
-        <f>(SUM(G20:G22)/3)</f>
+        <f t="shared" si="7"/>
         <v>1746856.3333333333</v>
       </c>
       <c r="H24" s="16">
-        <f>(SUM(H20:H22)/3)</f>
+        <f t="shared" si="7"/>
         <v>985984.66666666663</v>
       </c>
       <c r="I24" s="16">
-        <f>(SUM(I20:I22)/3)</f>
+        <f t="shared" si="7"/>
         <v>1746856.3333333333</v>
       </c>
     </row>

</xml_diff>